<commit_message>
faltaria hacer la perdida cuando no sale un numero se va reflejado colocar en el excel la ganancia de cada numero , se realizo el predictor nuevo orientado a objetos
</commit_message>
<xml_diff>
--- a/Data/Jugado.xlsx
+++ b/Data/Jugado.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonat\OneDrive\Escritorio\Repositorio\jonatha1992\Predictor_ruleta\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE338E3-F79C-4091-B2B9-B436E0D44093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77682FD7-00CA-4E3E-88FF-D96141D07C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -419,7 +419,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,32 +466,32 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E2">
         <f>C2*D2</f>
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="F2">
         <f>36*E2</f>
-        <v>3600</v>
+        <v>18000</v>
       </c>
       <c r="G2">
         <f>B2*E2</f>
-        <v>500</v>
+        <v>3500</v>
       </c>
       <c r="H2">
         <v>500</v>
       </c>
       <c r="I2">
         <f>F2-H2</f>
-        <v>3100</v>
+        <v>17500</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
@@ -499,33 +499,33 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E22" si="0">C3*D3</f>
-        <v>200</v>
+        <v>1000</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F22" si="1">36*E3</f>
-        <v>7200</v>
+        <v>36000</v>
       </c>
       <c r="G3">
         <f t="shared" ref="G3:G22" si="2">B3*E3</f>
-        <v>1000</v>
+        <v>7000</v>
       </c>
       <c r="H3">
         <f>G3+H2</f>
-        <v>1500</v>
+        <v>7500</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:I5" si="3">F3-H3</f>
-        <v>5700</v>
+        <v>28500</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -533,33 +533,33 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
       <c r="D4">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E4">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>1500</v>
       </c>
       <c r="F4">
         <f t="shared" si="1"/>
-        <v>10800</v>
+        <v>54000</v>
       </c>
       <c r="G4">
         <f t="shared" si="2"/>
-        <v>1500</v>
+        <v>10500</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H16" si="4">G4+H3</f>
-        <v>3000</v>
+        <v>18000</v>
       </c>
       <c r="I4">
-        <f t="shared" si="3"/>
-        <v>7800</v>
+        <f>F4-H4</f>
+        <v>36000</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
@@ -567,33 +567,33 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
       <c r="D5">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>72000</v>
       </c>
       <c r="G5">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="H5">
         <f t="shared" si="4"/>
-        <v>5000</v>
+        <v>32000</v>
       </c>
       <c r="I5">
         <f t="shared" si="3"/>
-        <v>9400</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
@@ -601,33 +601,33 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C6">
         <v>5</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E6">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="F6">
         <f t="shared" si="1"/>
-        <v>18000</v>
+        <v>90000</v>
       </c>
       <c r="G6">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>17500</v>
       </c>
       <c r="H6">
         <f t="shared" si="4"/>
-        <v>7500</v>
+        <v>49500</v>
       </c>
       <c r="I6">
         <f t="shared" ref="I6:I16" si="5">F6-H6</f>
-        <v>10500</v>
+        <v>40500</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -635,203 +635,203 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C7">
         <v>6</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>500</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>3000</v>
       </c>
       <c r="F7">
         <f t="shared" si="1"/>
-        <v>21600</v>
+        <v>108000</v>
       </c>
       <c r="G7">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>21000</v>
       </c>
       <c r="H7">
         <f t="shared" si="4"/>
-        <v>10500</v>
+        <v>70500</v>
       </c>
       <c r="I7">
         <f t="shared" si="5"/>
-        <v>11100</v>
+        <v>37500</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="2">
         <v>7</v>
       </c>
       <c r="D8">
-        <v>100</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="0"/>
-        <v>700</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>25200</v>
-      </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="0"/>
         <v>3500</v>
       </c>
-      <c r="H8">
+      <c r="F8" s="2">
+        <f t="shared" si="1"/>
+        <v>126000</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="2"/>
+        <v>24500</v>
+      </c>
+      <c r="H8" s="2">
         <f t="shared" si="4"/>
-        <v>14000</v>
-      </c>
-      <c r="I8">
+        <v>95000</v>
+      </c>
+      <c r="I8" s="2">
         <f t="shared" si="5"/>
-        <v>11200</v>
+        <v>31000</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>5</v>
-      </c>
-      <c r="C9">
+      <c r="A9" s="2">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>7</v>
+      </c>
+      <c r="C9" s="2">
         <v>8</v>
       </c>
       <c r="D9">
-        <v>100</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>800</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>28800</v>
-      </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="H9">
+      <c r="F9" s="2">
+        <f t="shared" si="1"/>
+        <v>144000</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="2"/>
+        <v>28000</v>
+      </c>
+      <c r="H9" s="2">
         <f t="shared" si="4"/>
-        <v>18000</v>
-      </c>
-      <c r="I9">
+        <v>123000</v>
+      </c>
+      <c r="I9" s="2">
         <f t="shared" si="5"/>
-        <v>10800</v>
+        <v>21000</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10">
+      <c r="A10" s="2">
         <v>8</v>
       </c>
-      <c r="B10">
-        <v>5</v>
-      </c>
-      <c r="C10">
+      <c r="B10" s="2">
+        <v>7</v>
+      </c>
+      <c r="C10" s="2">
         <v>9</v>
       </c>
       <c r="D10">
-        <v>100</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="0"/>
-        <v>900</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
-        <v>32400</v>
-      </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E10" s="2">
+        <f t="shared" si="0"/>
         <v>4500</v>
       </c>
-      <c r="H10">
+      <c r="F10" s="2">
+        <f t="shared" si="1"/>
+        <v>162000</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="2"/>
+        <v>31500</v>
+      </c>
+      <c r="H10" s="2">
         <f t="shared" si="4"/>
-        <v>22500</v>
-      </c>
-      <c r="I10">
+        <v>154500</v>
+      </c>
+      <c r="I10" s="2">
         <f t="shared" si="5"/>
-        <v>9900</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11">
+      <c r="A11" s="2">
         <v>9</v>
       </c>
-      <c r="B11">
-        <v>5</v>
-      </c>
-      <c r="C11">
+      <c r="B11" s="2">
+        <v>7</v>
+      </c>
+      <c r="C11" s="2">
         <v>10</v>
       </c>
       <c r="D11">
-        <v>100</v>
-      </c>
-      <c r="E11">
-        <f t="shared" si="0"/>
-        <v>1000</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
-        <v>36000</v>
-      </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E11" s="2">
+        <f t="shared" si="0"/>
         <v>5000</v>
       </c>
-      <c r="H11">
+      <c r="F11" s="2">
+        <f t="shared" si="1"/>
+        <v>180000</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="2"/>
+        <v>35000</v>
+      </c>
+      <c r="H11" s="2">
         <f t="shared" si="4"/>
-        <v>27500</v>
-      </c>
-      <c r="I11">
+        <v>189500</v>
+      </c>
+      <c r="I11" s="2">
         <f t="shared" si="5"/>
-        <v>8500</v>
+        <v>-9500</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12">
+      <c r="A12" s="2">
         <v>10</v>
       </c>
-      <c r="B12">
-        <v>5</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="2">
+        <v>7</v>
+      </c>
+      <c r="C12" s="2">
         <v>11</v>
       </c>
       <c r="D12">
-        <v>100</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>1100</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>39600</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+      <c r="E12" s="2">
+        <f t="shared" si="0"/>
         <v>5500</v>
       </c>
-      <c r="H12">
+      <c r="F12" s="2">
+        <f t="shared" si="1"/>
+        <v>198000</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="2"/>
+        <v>38500</v>
+      </c>
+      <c r="H12" s="2">
         <f t="shared" si="4"/>
-        <v>33000</v>
-      </c>
-      <c r="I12">
+        <v>228000</v>
+      </c>
+      <c r="I12" s="2">
         <f t="shared" si="5"/>
-        <v>6600</v>
+        <v>-30000</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -839,33 +839,33 @@
         <v>11</v>
       </c>
       <c r="B13" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C13" s="2">
         <v>4</v>
       </c>
-      <c r="D13" s="2">
-        <v>100</v>
+      <c r="D13">
+        <v>500</v>
       </c>
       <c r="E13" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>72000</v>
       </c>
       <c r="G13" s="2">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="H13" s="2">
         <f t="shared" si="4"/>
-        <v>35000</v>
+        <v>242000</v>
       </c>
       <c r="I13" s="2">
         <f t="shared" si="5"/>
-        <v>-20600</v>
+        <v>-170000</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
@@ -873,33 +873,33 @@
         <v>12</v>
       </c>
       <c r="B14" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C14" s="2">
         <v>4</v>
       </c>
-      <c r="D14" s="2">
-        <v>100</v>
+      <c r="D14">
+        <v>500</v>
       </c>
       <c r="E14" s="2">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2000</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="1"/>
-        <v>14400</v>
+        <v>72000</v>
       </c>
       <c r="G14" s="2">
         <f t="shared" si="2"/>
-        <v>2000</v>
+        <v>14000</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="4"/>
-        <v>37000</v>
+        <v>256000</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="5"/>
-        <v>-22600</v>
+        <v>-184000</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
@@ -907,33 +907,33 @@
         <v>13</v>
       </c>
       <c r="B15" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
       </c>
-      <c r="D15" s="2">
-        <v>100</v>
+      <c r="D15">
+        <v>500</v>
       </c>
       <c r="E15" s="2">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="1"/>
-        <v>18000</v>
+        <v>90000</v>
       </c>
       <c r="G15" s="2">
         <f t="shared" si="2"/>
-        <v>2500</v>
+        <v>17500</v>
       </c>
       <c r="H15" s="2">
         <f t="shared" si="4"/>
-        <v>39500</v>
+        <v>273500</v>
       </c>
       <c r="I15" s="2">
         <f t="shared" si="5"/>
-        <v>-21500</v>
+        <v>-183500</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
@@ -941,33 +941,33 @@
         <v>14</v>
       </c>
       <c r="B16" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2">
         <v>6</v>
       </c>
-      <c r="D16" s="2">
-        <v>100</v>
+      <c r="D16">
+        <v>500</v>
       </c>
       <c r="E16" s="2">
         <f t="shared" si="0"/>
-        <v>600</v>
+        <v>3000</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
-        <v>21600</v>
+        <v>108000</v>
       </c>
       <c r="G16" s="2">
         <f t="shared" si="2"/>
-        <v>3000</v>
+        <v>21000</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="4"/>
-        <v>42500</v>
+        <v>294500</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="5"/>
-        <v>-20900</v>
+        <v>-186500</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
@@ -975,33 +975,33 @@
         <v>15</v>
       </c>
       <c r="B17" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2">
         <v>7</v>
       </c>
-      <c r="D17" s="2">
-        <v>100</v>
+      <c r="D17">
+        <v>500</v>
       </c>
       <c r="E17" s="2">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>3500</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
-        <v>25200</v>
+        <v>126000</v>
       </c>
       <c r="G17" s="2">
         <f t="shared" si="2"/>
-        <v>3500</v>
+        <v>24500</v>
       </c>
       <c r="H17" s="2">
         <f t="shared" ref="H17:H21" si="6">G17+H16</f>
-        <v>46000</v>
+        <v>319000</v>
       </c>
       <c r="I17" s="2">
         <f t="shared" ref="I17:I21" si="7">F17-H17</f>
-        <v>-20800</v>
+        <v>-193000</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -1009,33 +1009,33 @@
         <v>16</v>
       </c>
       <c r="B18" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C18" s="2">
         <v>8</v>
       </c>
-      <c r="D18" s="2">
-        <v>100</v>
+      <c r="D18">
+        <v>500</v>
       </c>
       <c r="E18" s="2">
         <f t="shared" si="0"/>
-        <v>800</v>
+        <v>4000</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="1"/>
-        <v>28800</v>
+        <v>144000</v>
       </c>
       <c r="G18" s="2">
         <f t="shared" si="2"/>
-        <v>4000</v>
+        <v>28000</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="6"/>
-        <v>50000</v>
+        <v>347000</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="7"/>
-        <v>-21200</v>
+        <v>-203000</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
@@ -1043,33 +1043,33 @@
         <v>17</v>
       </c>
       <c r="B19" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" s="2">
         <v>9</v>
       </c>
-      <c r="D19" s="2">
-        <v>100</v>
+      <c r="D19">
+        <v>500</v>
       </c>
       <c r="E19" s="2">
         <f t="shared" si="0"/>
-        <v>900</v>
+        <v>4500</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="1"/>
-        <v>32400</v>
+        <v>162000</v>
       </c>
       <c r="G19" s="2">
         <f t="shared" si="2"/>
-        <v>4500</v>
+        <v>31500</v>
       </c>
       <c r="H19" s="2">
         <f t="shared" si="6"/>
-        <v>54500</v>
+        <v>378500</v>
       </c>
       <c r="I19" s="2">
         <f t="shared" si="7"/>
-        <v>-22100</v>
+        <v>-216500</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -1077,33 +1077,33 @@
         <v>18</v>
       </c>
       <c r="B20" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" s="2">
         <v>11</v>
       </c>
-      <c r="D20" s="2">
-        <v>100</v>
+      <c r="D20">
+        <v>500</v>
       </c>
       <c r="E20" s="2">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>5500</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="1"/>
-        <v>39600</v>
+        <v>198000</v>
       </c>
       <c r="G20" s="2">
         <f t="shared" si="2"/>
-        <v>5500</v>
+        <v>38500</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="6"/>
-        <v>60000</v>
+        <v>417000</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="7"/>
-        <v>-20400</v>
+        <v>-219000</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1111,33 +1111,33 @@
         <v>19</v>
       </c>
       <c r="B21" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C21" s="2">
         <v>13</v>
       </c>
-      <c r="D21" s="2">
-        <v>100</v>
+      <c r="D21">
+        <v>500</v>
       </c>
       <c r="E21" s="2">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>6500</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
-        <v>46800</v>
+        <v>234000</v>
       </c>
       <c r="G21" s="2">
         <f t="shared" si="2"/>
-        <v>6500</v>
+        <v>45500</v>
       </c>
       <c r="H21" s="2">
         <f t="shared" si="6"/>
-        <v>66500</v>
+        <v>462500</v>
       </c>
       <c r="I21" s="2">
         <f t="shared" si="7"/>
-        <v>-19700</v>
+        <v>-228500</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1145,33 +1145,33 @@
         <v>20</v>
       </c>
       <c r="B22" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C22" s="2">
         <v>15</v>
       </c>
-      <c r="D22" s="2">
-        <v>100</v>
+      <c r="D22">
+        <v>500</v>
       </c>
       <c r="E22" s="2">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>7500</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
-        <v>54000</v>
+        <v>270000</v>
       </c>
       <c r="G22" s="2">
         <f t="shared" si="2"/>
-        <v>7500</v>
+        <v>52500</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" ref="H22" si="8">G22+H21</f>
-        <v>74000</v>
+        <v>515000</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" ref="I22" si="9">F22-H22</f>
-        <v>-20000</v>
+        <v>-245000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>